<commit_message>
resolved comments except for fixture - not ready for merge yet
</commit_message>
<xml_diff>
--- a/tests/sample_data/valid_file.xlsx
+++ b/tests/sample_data/valid_file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/celia.maiorano/Python_Repositories/MoBI-Motion-Tracking-Development-branches/data_loader/mobi-motion-tracking/tests/sample_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28368EBC-34D1-2841-BAC6-DE5FEABD7794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628BA919-0A61-F247-874F-6BDF36C3AD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{46B6F311-2A56-6B4C-96B5-6A8ADC93E4E9}"/>
   </bookViews>
@@ -33,6 +33,32 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>x_Hip</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,14 +428,674 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338C41BB-6CC8-6547-9E15-478A16849207}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:BS17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+      <c r="R1">
+        <v>18</v>
+      </c>
+      <c r="S1">
+        <v>19</v>
+      </c>
+      <c r="T1">
+        <v>20</v>
+      </c>
+      <c r="U1">
+        <v>21</v>
+      </c>
+      <c r="V1">
+        <v>22</v>
+      </c>
+      <c r="W1">
+        <v>23</v>
+      </c>
+      <c r="X1">
+        <v>24</v>
+      </c>
+      <c r="Y1">
+        <v>25</v>
+      </c>
+      <c r="Z1">
+        <v>26</v>
+      </c>
+      <c r="AA1">
+        <v>27</v>
+      </c>
+      <c r="AB1">
+        <v>28</v>
+      </c>
+      <c r="AC1">
+        <v>29</v>
+      </c>
+      <c r="AD1">
+        <v>30</v>
+      </c>
+      <c r="AE1">
+        <v>31</v>
+      </c>
+      <c r="AF1">
+        <v>32</v>
+      </c>
+      <c r="AG1">
+        <v>33</v>
+      </c>
+      <c r="AH1">
+        <v>34</v>
+      </c>
+      <c r="AI1">
+        <v>35</v>
+      </c>
+      <c r="AJ1">
+        <v>36</v>
+      </c>
+      <c r="AK1">
+        <v>37</v>
+      </c>
+      <c r="AL1">
+        <v>38</v>
+      </c>
+      <c r="AM1">
+        <v>39</v>
+      </c>
+      <c r="AN1">
+        <v>40</v>
+      </c>
+      <c r="AO1">
+        <v>41</v>
+      </c>
+      <c r="AP1">
+        <v>42</v>
+      </c>
+      <c r="AQ1">
+        <v>43</v>
+      </c>
+      <c r="AR1">
+        <v>44</v>
+      </c>
+      <c r="AS1">
+        <v>45</v>
+      </c>
+      <c r="AT1">
+        <v>46</v>
+      </c>
+      <c r="AU1">
+        <v>47</v>
+      </c>
+      <c r="AV1">
+        <v>48</v>
+      </c>
+      <c r="AW1">
+        <v>49</v>
+      </c>
+      <c r="AX1">
+        <v>50</v>
+      </c>
+      <c r="AY1">
+        <v>51</v>
+      </c>
+      <c r="AZ1">
+        <v>52</v>
+      </c>
+      <c r="BA1">
+        <v>53</v>
+      </c>
+      <c r="BB1">
+        <v>54</v>
+      </c>
+      <c r="BC1">
+        <v>55</v>
+      </c>
+      <c r="BD1">
+        <v>56</v>
+      </c>
+      <c r="BE1">
+        <v>57</v>
+      </c>
+      <c r="BF1">
+        <v>58</v>
+      </c>
+      <c r="BG1">
+        <v>59</v>
+      </c>
+      <c r="BH1">
+        <v>60</v>
+      </c>
+      <c r="BI1">
+        <v>61</v>
+      </c>
+      <c r="BJ1">
+        <v>62</v>
+      </c>
+      <c r="BK1">
+        <v>63</v>
+      </c>
+      <c r="BL1">
+        <v>64</v>
+      </c>
+      <c r="BM1">
+        <v>65</v>
+      </c>
+      <c r="BN1">
+        <v>66</v>
+      </c>
+      <c r="BO1">
+        <v>67</v>
+      </c>
+      <c r="BP1">
+        <v>68</v>
+      </c>
+      <c r="BQ1">
+        <v>69</v>
+      </c>
+      <c r="BR1">
+        <v>70</v>
+      </c>
+      <c r="BS1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2">
+        <v>13</v>
+      </c>
+      <c r="N2">
+        <v>14</v>
+      </c>
+      <c r="O2">
+        <v>15</v>
+      </c>
+      <c r="P2">
+        <v>16</v>
+      </c>
+      <c r="Q2">
+        <v>17</v>
+      </c>
+      <c r="R2">
+        <v>18</v>
+      </c>
+      <c r="S2">
+        <v>19</v>
+      </c>
+      <c r="T2">
+        <v>20</v>
+      </c>
+      <c r="U2">
+        <v>21</v>
+      </c>
+      <c r="V2">
+        <v>22</v>
+      </c>
+      <c r="W2">
+        <v>23</v>
+      </c>
+      <c r="X2">
+        <v>24</v>
+      </c>
+      <c r="Y2">
+        <v>25</v>
+      </c>
+      <c r="Z2">
+        <v>26</v>
+      </c>
+      <c r="AA2">
+        <v>27</v>
+      </c>
+      <c r="AB2">
+        <v>28</v>
+      </c>
+      <c r="AC2">
+        <v>29</v>
+      </c>
+      <c r="AD2">
+        <v>30</v>
+      </c>
+      <c r="AE2">
+        <v>31</v>
+      </c>
+      <c r="AF2">
+        <v>32</v>
+      </c>
+      <c r="AG2">
+        <v>33</v>
+      </c>
+      <c r="AH2">
+        <v>34</v>
+      </c>
+      <c r="AI2">
+        <v>35</v>
+      </c>
+      <c r="AJ2">
+        <v>36</v>
+      </c>
+      <c r="AK2">
+        <v>37</v>
+      </c>
+      <c r="AL2">
+        <v>38</v>
+      </c>
+      <c r="AM2">
+        <v>39</v>
+      </c>
+      <c r="AN2">
+        <v>40</v>
+      </c>
+      <c r="AO2">
+        <v>41</v>
+      </c>
+      <c r="AP2">
+        <v>42</v>
+      </c>
+      <c r="AQ2">
+        <v>43</v>
+      </c>
+      <c r="AR2">
+        <v>44</v>
+      </c>
+      <c r="AS2">
+        <v>45</v>
+      </c>
+      <c r="AT2">
+        <v>46</v>
+      </c>
+      <c r="AU2">
+        <v>47</v>
+      </c>
+      <c r="AV2">
+        <v>48</v>
+      </c>
+      <c r="AW2">
+        <v>49</v>
+      </c>
+      <c r="AX2">
+        <v>50</v>
+      </c>
+      <c r="AY2">
+        <v>51</v>
+      </c>
+      <c r="AZ2">
+        <v>52</v>
+      </c>
+      <c r="BA2">
+        <v>53</v>
+      </c>
+      <c r="BB2">
+        <v>54</v>
+      </c>
+      <c r="BC2">
+        <v>55</v>
+      </c>
+      <c r="BD2">
+        <v>56</v>
+      </c>
+      <c r="BE2">
+        <v>57</v>
+      </c>
+      <c r="BF2">
+        <v>58</v>
+      </c>
+      <c r="BG2">
+        <v>59</v>
+      </c>
+      <c r="BH2">
+        <v>60</v>
+      </c>
+      <c r="BI2">
+        <v>61</v>
+      </c>
+      <c r="BJ2">
+        <v>62</v>
+      </c>
+      <c r="BK2">
+        <v>63</v>
+      </c>
+      <c r="BL2">
+        <v>64</v>
+      </c>
+      <c r="BM2">
+        <v>65</v>
+      </c>
+      <c r="BN2">
+        <v>66</v>
+      </c>
+      <c r="BO2">
+        <v>67</v>
+      </c>
+      <c r="BP2">
+        <v>68</v>
+      </c>
+      <c r="BQ2">
+        <v>69</v>
+      </c>
+      <c r="BR2">
+        <v>70</v>
+      </c>
+      <c r="BS2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>71</v>
+      </c>
+      <c r="B3">
+        <v>72</v>
+      </c>
+      <c r="C3">
+        <v>73</v>
+      </c>
+      <c r="D3">
+        <v>74</v>
+      </c>
+      <c r="E3">
+        <v>75</v>
+      </c>
+      <c r="F3">
+        <v>76</v>
+      </c>
+      <c r="G3">
+        <v>77</v>
+      </c>
+      <c r="H3">
+        <v>78</v>
+      </c>
+      <c r="I3">
+        <v>79</v>
+      </c>
+      <c r="J3">
+        <v>80</v>
+      </c>
+      <c r="K3">
+        <v>81</v>
+      </c>
+      <c r="L3">
+        <v>82</v>
+      </c>
+      <c r="M3">
+        <v>83</v>
+      </c>
+      <c r="N3">
+        <v>84</v>
+      </c>
+      <c r="O3">
+        <v>85</v>
+      </c>
+      <c r="P3">
+        <v>86</v>
+      </c>
+      <c r="Q3">
+        <v>87</v>
+      </c>
+      <c r="R3">
+        <v>88</v>
+      </c>
+      <c r="S3">
+        <v>89</v>
+      </c>
+      <c r="T3">
+        <v>90</v>
+      </c>
+      <c r="U3">
+        <v>91</v>
+      </c>
+      <c r="V3">
+        <v>92</v>
+      </c>
+      <c r="W3">
+        <v>93</v>
+      </c>
+      <c r="X3">
+        <v>94</v>
+      </c>
+      <c r="Y3">
+        <v>95</v>
+      </c>
+      <c r="Z3">
+        <v>96</v>
+      </c>
+      <c r="AA3">
+        <v>97</v>
+      </c>
+      <c r="AB3">
+        <v>98</v>
+      </c>
+      <c r="AC3">
+        <v>99</v>
+      </c>
+      <c r="AD3">
+        <v>100</v>
+      </c>
+      <c r="AE3">
+        <v>101</v>
+      </c>
+      <c r="AF3">
+        <v>102</v>
+      </c>
+      <c r="AG3">
+        <v>103</v>
+      </c>
+      <c r="AH3">
+        <v>104</v>
+      </c>
+      <c r="AI3">
+        <v>105</v>
+      </c>
+      <c r="AJ3">
+        <v>106</v>
+      </c>
+      <c r="AK3">
+        <v>107</v>
+      </c>
+      <c r="AL3">
+        <v>108</v>
+      </c>
+      <c r="AM3">
+        <v>109</v>
+      </c>
+      <c r="AN3">
+        <v>110</v>
+      </c>
+      <c r="AO3">
+        <v>111</v>
+      </c>
+      <c r="AP3">
+        <v>112</v>
+      </c>
+      <c r="AQ3">
+        <v>113</v>
+      </c>
+      <c r="AR3">
+        <v>114</v>
+      </c>
+      <c r="AS3">
+        <v>115</v>
+      </c>
+      <c r="AT3">
+        <v>116</v>
+      </c>
+      <c r="AU3">
+        <v>117</v>
+      </c>
+      <c r="AV3">
+        <v>118</v>
+      </c>
+      <c r="AW3">
+        <v>119</v>
+      </c>
+      <c r="AX3">
+        <v>120</v>
+      </c>
+      <c r="AY3">
+        <v>121</v>
+      </c>
+      <c r="AZ3">
+        <v>122</v>
+      </c>
+      <c r="BA3">
+        <v>123</v>
+      </c>
+      <c r="BB3">
+        <v>124</v>
+      </c>
+      <c r="BC3">
+        <v>125</v>
+      </c>
+      <c r="BD3">
+        <v>126</v>
+      </c>
+      <c r="BE3">
+        <v>127</v>
+      </c>
+      <c r="BF3">
+        <v>128</v>
+      </c>
+      <c r="BG3">
+        <v>129</v>
+      </c>
+      <c r="BH3">
+        <v>130</v>
+      </c>
+      <c r="BI3">
+        <v>131</v>
+      </c>
+      <c r="BJ3">
+        <v>132</v>
+      </c>
+      <c r="BK3">
+        <v>133</v>
+      </c>
+      <c r="BL3">
+        <v>134</v>
+      </c>
+      <c r="BM3">
+        <v>135</v>
+      </c>
+      <c r="BN3">
+        <v>136</v>
+      </c>
+      <c r="BO3">
+        <v>137</v>
+      </c>
+      <c r="BP3">
+        <v>138</v>
+      </c>
+      <c r="BQ3">
+        <v>139</v>
+      </c>
+      <c r="BR3">
+        <v>140</v>
+      </c>
+      <c r="BS3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:71" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>